<commit_message>
Fix 'is' and doctype == 'is' bug
</commit_message>
<xml_diff>
--- a/plan/Finance statements fields.xlsx
+++ b/plan/Finance statements fields.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="105">
   <si>
     <t>APPLE INC  (AAPL) CashFlowFlag BALANCE SHEET</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>Derivative liabilities</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Fiscal year end</t>
   </si>
 </sst>
 </file>
@@ -701,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.33203125" defaultRowHeight="77" customHeight="1" x14ac:dyDescent="0"/>
@@ -712,7 +718,7 @@
     <col min="1" max="16384" width="20.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="77" customHeight="1">
+    <row r="1" spans="1:18" ht="77" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,8 +767,11 @@
       <c r="P1" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="77" customHeight="1">
+      <c r="R1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="77" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -811,8 +820,11 @@
       <c r="P2" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="77" customHeight="1">
+      <c r="R2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="77" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -862,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="77" customHeight="1">
+    <row r="4" spans="1:18" ht="77" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -912,7 +924,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="77" customHeight="1">
+    <row r="5" spans="1:18" ht="77" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -962,7 +974,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="77" customHeight="1">
+    <row r="6" spans="1:18" ht="77" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1024,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="77" customHeight="1">
+    <row r="7" spans="1:18" ht="77" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1062,7 +1074,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="77" customHeight="1">
+    <row r="8" spans="1:18" ht="77" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1112,7 +1124,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="77" customHeight="1">
+    <row r="9" spans="1:18" ht="77" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="77" customHeight="1">
+    <row r="10" spans="1:18" ht="77" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1212,7 +1224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="77" customHeight="1">
+    <row r="11" spans="1:18" ht="77" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="77" customHeight="1">
+    <row r="12" spans="1:18" ht="77" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1312,7 +1324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="77" customHeight="1">
+    <row r="13" spans="1:18" ht="77" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="77" customHeight="1">
+    <row r="14" spans="1:18" ht="77" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="77" customHeight="1">
+    <row r="15" spans="1:18" ht="77" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1462,7 +1474,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="77" customHeight="1">
+    <row r="16" spans="1:18" ht="77" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>